<commit_message>
Add thumbnails, documentation, and update reports with thumbnail paths
Co-authored-by: Ali5829511 <132597948+Ali5829511@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/data/ParkPow_Licenses_Report.xlsx
+++ b/data/ParkPow_Licenses_Report.xlsx
@@ -489,7 +489,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>لا توجد صورة</t>
+          <t>assets/parkpow_thumbnails/thumbnail_6nBNl5S6L6w.jpg</t>
         </is>
       </c>
     </row>
@@ -517,7 +517,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>لا توجد صورة</t>
+          <t>assets/parkpow_thumbnails/thumbnail_A7xMk9P2Q3r.jpg</t>
         </is>
       </c>
     </row>
@@ -545,7 +545,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>لا توجد صورة</t>
+          <t>assets/parkpow_thumbnails/thumbnail_B4cNt8R1S5v.jpg</t>
         </is>
       </c>
     </row>

</xml_diff>